<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@7754791925437dacf85bd36af3826fdeca948c29 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O396"/>
+  <dimension ref="A1:O405"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21868,6 +21868,495 @@
       <c r="N396" t="inlineStr"/>
       <c r="O396" t="inlineStr"/>
     </row>
+    <row r="397">
+      <c r="A397" s="1" t="n">
+        <v>395</v>
+      </c>
+      <c r="B397" s="2" t="n">
+        <v>44246.55214344907</v>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Turku</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F397" t="n">
+        <v>8</v>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H397" t="n">
+        <v>1</v>
+      </c>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer (Backend)</t>
+        </is>
+      </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="K397" t="n">
+        <v>5700</v>
+      </c>
+      <c r="L397" t="n">
+        <v>74100</v>
+      </c>
+      <c r="M397" t="b">
+        <v>1</v>
+      </c>
+      <c r="N397" t="inlineStr"/>
+      <c r="O397" t="inlineStr">
+        <is>
+          <t>Ennen koronaa oli osittainen etätyö, koronan jälkeen 100%</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1" t="n">
+        <v>396</v>
+      </c>
+      <c r="B398" s="2" t="n">
+        <v>44246.55232758102</v>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F398" t="n">
+        <v>3</v>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H398" t="n">
+        <v>1</v>
+      </c>
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="J398" t="inlineStr"/>
+      <c r="K398" t="n">
+        <v>3200</v>
+      </c>
+      <c r="L398" t="n">
+        <v>40000</v>
+      </c>
+      <c r="M398" t="b">
+        <v>0</v>
+      </c>
+      <c r="N398" t="inlineStr"/>
+      <c r="O398" t="inlineStr"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="1" t="n">
+        <v>397</v>
+      </c>
+      <c r="B399" s="2" t="n">
+        <v>44246.56990268519</v>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>Jyväskylä</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F399" t="n">
+        <v>6</v>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H399" t="n">
+        <v>1</v>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>WordPress / Frontend-koodari</t>
+        </is>
+      </c>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="K399" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L399" t="n">
+        <v>37500</v>
+      </c>
+      <c r="M399" t="b">
+        <v>1</v>
+      </c>
+      <c r="N399" t="inlineStr"/>
+      <c r="O399" t="inlineStr"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="B400" s="2" t="n">
+        <v>44246.58209564815</v>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>Jyväskylä</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>21-25 v</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F400" t="n">
+        <v>21</v>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H400" t="n">
+        <v>1</v>
+      </c>
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>Arkkitehti</t>
+        </is>
+      </c>
+      <c r="J400" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="K400" t="n">
+        <v>5500</v>
+      </c>
+      <c r="L400" t="n">
+        <v>75000</v>
+      </c>
+      <c r="M400" t="b">
+        <v>1</v>
+      </c>
+      <c r="N400" t="inlineStr"/>
+      <c r="O400" t="inlineStr"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="n">
+        <v>399</v>
+      </c>
+      <c r="B401" s="2" t="n">
+        <v>44246.58394819444</v>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F401" t="n">
+        <v>7</v>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H401" t="n">
+        <v>1</v>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä, backend</t>
+        </is>
+      </c>
+      <c r="J401" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="K401" t="n">
+        <v>5470</v>
+      </c>
+      <c r="L401" t="n">
+        <v>94000</v>
+      </c>
+      <c r="M401" t="b">
+        <v>1</v>
+      </c>
+      <c r="N401" t="inlineStr"/>
+      <c r="O401" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="B402" s="2" t="n">
+        <v>44246.58876788194</v>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr"/>
+      <c r="F402" t="n">
+        <v>3</v>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H402" t="n">
+        <v>1</v>
+      </c>
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>Full stack developer</t>
+        </is>
+      </c>
+      <c r="J402" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="K402" t="n">
+        <v>5300</v>
+      </c>
+      <c r="L402" t="n">
+        <v>66250</v>
+      </c>
+      <c r="M402" t="b">
+        <v>1</v>
+      </c>
+      <c r="N402" t="inlineStr"/>
+      <c r="O402" t="inlineStr"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="n">
+        <v>401</v>
+      </c>
+      <c r="B403" s="2" t="n">
+        <v>44246.59057026621</v>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>Kuopio</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F403" t="n">
+        <v>9</v>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H403" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>CTO</t>
+        </is>
+      </c>
+      <c r="J403" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="K403" t="n">
+        <v>5200</v>
+      </c>
+      <c r="L403" t="n">
+        <v>65000</v>
+      </c>
+      <c r="M403" t="b">
+        <v>1</v>
+      </c>
+      <c r="N403" t="inlineStr"/>
+      <c r="O403" t="inlineStr"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="1" t="n">
+        <v>402</v>
+      </c>
+      <c r="B404" s="2" t="n">
+        <v>44246.59166526621</v>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F404" t="n">
+        <v>14</v>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H404" t="n">
+        <v>1</v>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>Projektipäällikkö</t>
+        </is>
+      </c>
+      <c r="J404" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="K404" t="n">
+        <v>6400</v>
+      </c>
+      <c r="L404" t="n">
+        <v>102000</v>
+      </c>
+      <c r="M404" t="b">
+        <v>1</v>
+      </c>
+      <c r="N404" t="inlineStr"/>
+      <c r="O404" t="inlineStr"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="1" t="n">
+        <v>403</v>
+      </c>
+      <c r="B405" s="2" t="n">
+        <v>44246.60321177083</v>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="F405" t="n">
+        <v>15</v>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="H405" t="n">
+        <v>1</v>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>Frontend &amp; UX</t>
+        </is>
+      </c>
+      <c r="J405" t="inlineStr"/>
+      <c r="K405" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L405" t="inlineStr">
+        <is>
+          <t>Optiot</t>
+        </is>
+      </c>
+      <c r="M405" t="b">
+        <v>0</v>
+      </c>
+      <c r="N405" t="inlineStr"/>
+      <c r="O405" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@61093bde65514dc161c997be472841376d0de220 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N411"/>
+  <dimension ref="A1:N412"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -568,7 +568,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -920,7 +920,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>30-35 v</t>
+          <t>31-35 v</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -21441,6 +21441,54 @@
       <c r="M411" t="inlineStr"/>
       <c r="N411" t="inlineStr"/>
     </row>
+    <row r="412">
+      <c r="A412" s="2" t="n">
+        <v>44246.62593082176</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Turku</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E412" t="n">
+        <v>9</v>
+      </c>
+      <c r="F412" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G412" t="n">
+        <v>1</v>
+      </c>
+      <c r="H412" t="inlineStr">
+        <is>
+          <t>Full-stack ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I412" t="inlineStr"/>
+      <c r="J412" t="n">
+        <v>3900</v>
+      </c>
+      <c r="K412" t="n">
+        <v>52000</v>
+      </c>
+      <c r="L412" t="b">
+        <v>0</v>
+      </c>
+      <c r="M412" t="inlineStr"/>
+      <c r="N412" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@ef70a3ae1b1faa16727e78d0280716ebc831361f 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N412"/>
+  <dimension ref="A1:N417"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21489,6 +21489,282 @@
       <c r="M412" t="inlineStr"/>
       <c r="N412" t="inlineStr"/>
     </row>
+    <row r="413">
+      <c r="A413" s="2" t="n">
+        <v>44246.62923952546</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E413" t="n">
+        <v>14</v>
+      </c>
+      <c r="F413" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G413" t="n">
+        <v>1</v>
+      </c>
+      <c r="H413" t="inlineStr">
+        <is>
+          <t>Senior consultant</t>
+        </is>
+      </c>
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J413" t="n">
+        <v>8500</v>
+      </c>
+      <c r="K413" t="n">
+        <v>100000</v>
+      </c>
+      <c r="L413" t="b">
+        <v>1</v>
+      </c>
+      <c r="M413" t="inlineStr">
+        <is>
+          <t>Sulava</t>
+        </is>
+      </c>
+      <c r="N413" t="inlineStr"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="2" t="n">
+        <v>44246.63462665509</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Pori</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E414" t="n">
+        <v>8</v>
+      </c>
+      <c r="F414" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G414" t="n">
+        <v>1</v>
+      </c>
+      <c r="H414" t="inlineStr">
+        <is>
+          <t>Tech Lead</t>
+        </is>
+      </c>
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J414" t="n">
+        <v>5080</v>
+      </c>
+      <c r="K414" t="n">
+        <v>65000</v>
+      </c>
+      <c r="L414" t="b">
+        <v>0</v>
+      </c>
+      <c r="M414" t="inlineStr">
+        <is>
+          <t>Iso konsulttitalo</t>
+        </is>
+      </c>
+      <c r="N414" t="inlineStr">
+        <is>
+          <t>Sijainti Pori, mutta etätöitä 100%. Varsinainen positio Tampere - Helsinki. Edut aika huonot, perusjutut. Työ itsessään aika masentavaa. Seuraavaksi varmaan freelance/yrittäjyys.</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="2" t="n">
+        <v>44246.64167922454</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E415" t="n">
+        <v>14</v>
+      </c>
+      <c r="F415" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G415" t="n">
+        <v>1</v>
+      </c>
+      <c r="H415" t="inlineStr">
+        <is>
+          <t>Ohjelmistotestaaja</t>
+        </is>
+      </c>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J415" t="n">
+        <v>4100</v>
+      </c>
+      <c r="K415" t="n">
+        <v>55000</v>
+      </c>
+      <c r="L415" t="b">
+        <v>1</v>
+      </c>
+      <c r="M415" t="inlineStr"/>
+      <c r="N415" t="inlineStr"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="2" t="n">
+        <v>44246.64923311343</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>muu</t>
+        </is>
+      </c>
+      <c r="E416" t="n">
+        <v>7</v>
+      </c>
+      <c r="F416" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G416" t="n">
+        <v>1</v>
+      </c>
+      <c r="H416" t="inlineStr">
+        <is>
+          <t>Full-stack developer</t>
+        </is>
+      </c>
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J416" t="n">
+        <v>5550</v>
+      </c>
+      <c r="K416" t="n">
+        <v>69400</v>
+      </c>
+      <c r="L416" t="b">
+        <v>1</v>
+      </c>
+      <c r="M416" t="inlineStr"/>
+      <c r="N416" t="inlineStr"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="2" t="n">
+        <v>44246.65296685185</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E417" t="n">
+        <v>5</v>
+      </c>
+      <c r="F417" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G417" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H417" t="inlineStr">
+        <is>
+          <t>Full-stack/mobiili/design</t>
+        </is>
+      </c>
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J417" t="n">
+        <v>7000</v>
+      </c>
+      <c r="K417" t="n">
+        <v>90000</v>
+      </c>
+      <c r="L417" t="b">
+        <v>1</v>
+      </c>
+      <c r="M417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mavericks </t>
+        </is>
+      </c>
+      <c r="N417" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@3535d14330917fea2e0543ac6ae3f9218c20a70f 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N417"/>
+  <dimension ref="A1:N418"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21765,6 +21765,58 @@
       </c>
       <c r="N417" t="inlineStr"/>
     </row>
+    <row r="418">
+      <c r="A418" s="2" t="n">
+        <v>44246.67002717593</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E418" t="n">
+        <v>16</v>
+      </c>
+      <c r="F418" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G418" t="n">
+        <v>1</v>
+      </c>
+      <c r="H418" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I418" t="inlineStr"/>
+      <c r="J418" t="n">
+        <v>4800</v>
+      </c>
+      <c r="K418" t="n">
+        <v>65000</v>
+      </c>
+      <c r="L418" t="b">
+        <v>1</v>
+      </c>
+      <c r="M418" t="inlineStr"/>
+      <c r="N418" t="inlineStr">
+        <is>
+          <t>Bonukset riippuu firman tuloksesta. Palkka olisi varmastikin enemmän muualla mutta uskoakseni linjassa kollegoideni kanssa.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@496541e477d9832426f3c6b04808d89f6ec1a8b6 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N418"/>
+  <dimension ref="A1:N420"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -21817,6 +21817,112 @@
         </is>
       </c>
     </row>
+    <row r="419">
+      <c r="A419" s="2" t="n">
+        <v>44246.67881818287</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E419" t="n">
+        <v>8</v>
+      </c>
+      <c r="F419" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G419" t="inlineStr"/>
+      <c r="H419" t="inlineStr">
+        <is>
+          <t>Product Owner</t>
+        </is>
+      </c>
+      <c r="I419" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J419" t="n">
+        <v>4500</v>
+      </c>
+      <c r="K419" t="n">
+        <v>56200</v>
+      </c>
+      <c r="L419" t="b">
+        <v>1</v>
+      </c>
+      <c r="M419" t="inlineStr"/>
+      <c r="N419" t="inlineStr"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="2" t="n">
+        <v>44246.68510069444</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E420" t="n">
+        <v>16</v>
+      </c>
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G420" t="n">
+        <v>1</v>
+      </c>
+      <c r="H420" t="inlineStr">
+        <is>
+          <t>Mobile SW</t>
+        </is>
+      </c>
+      <c r="I420" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J420" t="n">
+        <v>8000</v>
+      </c>
+      <c r="K420" t="n">
+        <v>95000</v>
+      </c>
+      <c r="L420" t="b">
+        <v>1</v>
+      </c>
+      <c r="M420" t="inlineStr">
+        <is>
+          <t>Mavericks</t>
+        </is>
+      </c>
+      <c r="N420" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@52114a5f9520191c6e5b88ad528725aa01e34fbf 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N420"/>
+  <dimension ref="A1:N425"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21923,6 +21923,276 @@
       </c>
       <c r="N420" t="inlineStr"/>
     </row>
+    <row r="421">
+      <c r="A421" s="2" t="n">
+        <v>44246.68990465278</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E421" t="n">
+        <v>11</v>
+      </c>
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G421" t="n">
+        <v>1</v>
+      </c>
+      <c r="H421" t="inlineStr">
+        <is>
+          <t>Full stack</t>
+        </is>
+      </c>
+      <c r="I421" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J421" t="n">
+        <v>7000</v>
+      </c>
+      <c r="K421" t="n">
+        <v>87500</v>
+      </c>
+      <c r="L421" t="b">
+        <v>1</v>
+      </c>
+      <c r="M421" t="inlineStr">
+        <is>
+          <t>Mavericks</t>
+        </is>
+      </c>
+      <c r="N421" t="inlineStr"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="2" t="n">
+        <v>44246.69036510416</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E422" t="n">
+        <v>12</v>
+      </c>
+      <c r="F422" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G422" t="n">
+        <v>1</v>
+      </c>
+      <c r="H422" t="inlineStr">
+        <is>
+          <t>full-stack</t>
+        </is>
+      </c>
+      <c r="I422" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J422" t="n">
+        <v>8000</v>
+      </c>
+      <c r="K422" t="n">
+        <v>95000</v>
+      </c>
+      <c r="L422" t="b">
+        <v>1</v>
+      </c>
+      <c r="M422" t="inlineStr">
+        <is>
+          <t>Mavericks</t>
+        </is>
+      </c>
+      <c r="N422" t="inlineStr"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="2" t="n">
+        <v>44246.69231409722</v>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>41-45 v</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E423" t="n">
+        <v>22</v>
+      </c>
+      <c r="F423" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G423" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H423" t="inlineStr">
+        <is>
+          <t>ohjelmistokehittäjä (backend) / arkkitehti</t>
+        </is>
+      </c>
+      <c r="I423" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J423" t="n">
+        <v>4700</v>
+      </c>
+      <c r="K423" t="n">
+        <v>58750</v>
+      </c>
+      <c r="L423" t="b">
+        <v>0</v>
+      </c>
+      <c r="M423" t="inlineStr"/>
+      <c r="N423" t="inlineStr"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="2" t="n">
+        <v>44246.69353475695</v>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E424" t="n">
+        <v>2</v>
+      </c>
+      <c r="F424" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G424" t="n">
+        <v>1</v>
+      </c>
+      <c r="H424" t="inlineStr">
+        <is>
+          <t>WordPress-kehittäjä</t>
+        </is>
+      </c>
+      <c r="I424" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J424" t="n">
+        <v>3000</v>
+      </c>
+      <c r="K424" t="n">
+        <v>37500</v>
+      </c>
+      <c r="L424" t="b">
+        <v>0</v>
+      </c>
+      <c r="M424" t="inlineStr"/>
+      <c r="N424" t="inlineStr"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="2" t="n">
+        <v>44246.69392165509</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E425" t="n">
+        <v>5</v>
+      </c>
+      <c r="F425" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G425" t="n">
+        <v>1</v>
+      </c>
+      <c r="H425" t="inlineStr">
+        <is>
+          <t>Data scientist</t>
+        </is>
+      </c>
+      <c r="I425" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J425" t="n">
+        <v>4300</v>
+      </c>
+      <c r="K425" t="n">
+        <v>53750</v>
+      </c>
+      <c r="L425" t="inlineStr"/>
+      <c r="M425" t="inlineStr">
+        <is>
+          <t>Wapice</t>
+        </is>
+      </c>
+      <c r="N425" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@41a54d0c6cfa9f90cefd5cd4b5dec420205c3959 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N425"/>
+  <dimension ref="A1:N426"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22193,6 +22193,60 @@
       </c>
       <c r="N425" t="inlineStr"/>
     </row>
+    <row r="426">
+      <c r="A426" s="2" t="n">
+        <v>44246.70005435185</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>41-45 v</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E426" t="n">
+        <v>15</v>
+      </c>
+      <c r="F426" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G426" t="n">
+        <v>1</v>
+      </c>
+      <c r="H426" t="inlineStr">
+        <is>
+          <t>ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I426" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J426" t="inlineStr">
+        <is>
+          <t>7500+</t>
+        </is>
+      </c>
+      <c r="K426" t="n">
+        <v>100000</v>
+      </c>
+      <c r="L426" t="b">
+        <v>1</v>
+      </c>
+      <c r="M426" t="inlineStr"/>
+      <c r="N426" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@6e3456c12b8c9eec17845d1ec45422cfe61cae4f 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N426"/>
+  <dimension ref="A1:N429"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22247,6 +22247,158 @@
       <c r="M426" t="inlineStr"/>
       <c r="N426" t="inlineStr"/>
     </row>
+    <row r="427">
+      <c r="A427" s="2" t="n">
+        <v>44246.70452188658</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Turku</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E427" t="n">
+        <v>13</v>
+      </c>
+      <c r="F427" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G427" t="n">
+        <v>1</v>
+      </c>
+      <c r="H427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lead Software Engineer </t>
+        </is>
+      </c>
+      <c r="I427" t="inlineStr"/>
+      <c r="J427" t="n">
+        <v>5500</v>
+      </c>
+      <c r="K427" t="n">
+        <v>75000</v>
+      </c>
+      <c r="L427" t="b">
+        <v>1</v>
+      </c>
+      <c r="M427" t="inlineStr"/>
+      <c r="N427" t="inlineStr"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="2" t="n">
+        <v>44246.71758012731</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E428" t="n">
+        <v>15</v>
+      </c>
+      <c r="F428" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G428" t="n">
+        <v>1</v>
+      </c>
+      <c r="H428" t="inlineStr">
+        <is>
+          <t>full-stack</t>
+        </is>
+      </c>
+      <c r="I428" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J428" t="n">
+        <v>6000</v>
+      </c>
+      <c r="K428" t="n">
+        <v>76000</v>
+      </c>
+      <c r="L428" t="b">
+        <v>1</v>
+      </c>
+      <c r="M428" t="inlineStr"/>
+      <c r="N428" t="inlineStr"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="2" t="n">
+        <v>44246.74418030093</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>21-25 v</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E429" t="n">
+        <v>4</v>
+      </c>
+      <c r="F429" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G429" t="n">
+        <v>1</v>
+      </c>
+      <c r="H429" t="inlineStr">
+        <is>
+          <t>Frontend ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I429" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J429" t="n">
+        <v>4000</v>
+      </c>
+      <c r="K429" t="n">
+        <v>55000</v>
+      </c>
+      <c r="L429" t="b">
+        <v>1</v>
+      </c>
+      <c r="M429" t="inlineStr"/>
+      <c r="N429" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@b75edb5dc30cc82412a27432979bea072893b51e 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O431"/>
+  <dimension ref="A1:O458"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24352,6 +24352,1499 @@
         <v>3125</v>
       </c>
     </row>
+    <row r="432">
+      <c r="A432" s="2" t="n">
+        <v>44246.79140840278</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E432" t="n">
+        <v>5</v>
+      </c>
+      <c r="F432" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G432" t="n">
+        <v>1</v>
+      </c>
+      <c r="H432" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I432" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J432" t="n">
+        <v>4200</v>
+      </c>
+      <c r="K432" t="n">
+        <v>52500</v>
+      </c>
+      <c r="L432" t="b">
+        <v>1</v>
+      </c>
+      <c r="M432" t="inlineStr"/>
+      <c r="N432" t="inlineStr"/>
+      <c r="O432" t="n">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="2" t="n">
+        <v>44246.80164439815</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Vaasa</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>41-45 v</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E433" t="n">
+        <v>20</v>
+      </c>
+      <c r="F433" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G433" t="n">
+        <v>1</v>
+      </c>
+      <c r="H433" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I433" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J433" t="n">
+        <v>4250</v>
+      </c>
+      <c r="K433" t="n">
+        <v>55000</v>
+      </c>
+      <c r="L433" t="b">
+        <v>0</v>
+      </c>
+      <c r="M433" t="inlineStr"/>
+      <c r="N433" t="inlineStr"/>
+      <c r="O433" t="n">
+        <v>4583.333333333333</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="2" t="n">
+        <v>44246.82285515047</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Turku</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>21-25 v</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E434" t="n">
+        <v>2</v>
+      </c>
+      <c r="F434" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G434" t="inlineStr"/>
+      <c r="H434" t="inlineStr"/>
+      <c r="I434" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J434" t="n">
+        <v>3300</v>
+      </c>
+      <c r="K434" t="n">
+        <v>41250</v>
+      </c>
+      <c r="L434" t="inlineStr"/>
+      <c r="M434" t="inlineStr"/>
+      <c r="N434" t="inlineStr"/>
+      <c r="O434" t="n">
+        <v>3437.5</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="2" t="n">
+        <v>44246.87332728009</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E435" t="n">
+        <v>6</v>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G435" t="n">
+        <v>1</v>
+      </c>
+      <c r="H435" t="inlineStr">
+        <is>
+          <t>Lead developer</t>
+        </is>
+      </c>
+      <c r="I435" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J435" t="n">
+        <v>4500</v>
+      </c>
+      <c r="K435" t="n">
+        <v>56250</v>
+      </c>
+      <c r="L435" t="b">
+        <v>1</v>
+      </c>
+      <c r="M435" t="inlineStr"/>
+      <c r="N435" t="inlineStr"/>
+      <c r="O435" t="n">
+        <v>4687.5</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="2" t="n">
+        <v>44246.87344513889</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E436" t="n">
+        <v>6</v>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G436" t="n">
+        <v>1</v>
+      </c>
+      <c r="H436" t="inlineStr"/>
+      <c r="I436" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J436" t="n">
+        <v>4250</v>
+      </c>
+      <c r="K436" t="n">
+        <v>53000</v>
+      </c>
+      <c r="L436" t="b">
+        <v>1</v>
+      </c>
+      <c r="M436" t="inlineStr"/>
+      <c r="N436" t="inlineStr"/>
+      <c r="O436" t="n">
+        <v>4416.666666666667</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="2" t="n">
+        <v>44246.90860390046</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>21-25 v</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E437" t="n">
+        <v>2</v>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G437" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>Ful-stack kehittäjä front-end painolla</t>
+        </is>
+      </c>
+      <c r="I437" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J437" t="n">
+        <v>3300</v>
+      </c>
+      <c r="K437" t="n">
+        <v>41250</v>
+      </c>
+      <c r="L437" t="b">
+        <v>0</v>
+      </c>
+      <c r="M437" t="inlineStr">
+        <is>
+          <t>Bitwise Oy</t>
+        </is>
+      </c>
+      <c r="N437" t="inlineStr"/>
+      <c r="O437" t="n">
+        <v>3437.5</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="2" t="n">
+        <v>44247.27491872685</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E438" t="n">
+        <v>7</v>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G438" t="n">
+        <v>1</v>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>Full-Stack</t>
+        </is>
+      </c>
+      <c r="I438" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J438" t="n">
+        <v>6750</v>
+      </c>
+      <c r="K438" t="n">
+        <v>85000</v>
+      </c>
+      <c r="L438" t="b">
+        <v>1</v>
+      </c>
+      <c r="M438" t="inlineStr"/>
+      <c r="N438" t="inlineStr"/>
+      <c r="O438" t="n">
+        <v>7083.333333333333</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="2" t="n">
+        <v>44247.34909702546</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E439" t="n">
+        <v>5</v>
+      </c>
+      <c r="F439" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G439" t="n">
+        <v>1</v>
+      </c>
+      <c r="H439" t="inlineStr">
+        <is>
+          <t>Konsultti / Full stack / Tech lead</t>
+        </is>
+      </c>
+      <c r="I439" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J439" t="n">
+        <v>9300</v>
+      </c>
+      <c r="K439" t="n">
+        <v>115000</v>
+      </c>
+      <c r="L439" t="b">
+        <v>1</v>
+      </c>
+      <c r="M439" t="inlineStr">
+        <is>
+          <t>Mavericks Software Oy</t>
+        </is>
+      </c>
+      <c r="N439" t="inlineStr"/>
+      <c r="O439" t="n">
+        <v>9583.333333333334</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="2" t="n">
+        <v>44247.39400061343</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>41-45 v</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E440" t="n">
+        <v>16</v>
+      </c>
+      <c r="F440" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G440" t="n">
+        <v>1</v>
+      </c>
+      <c r="H440" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä (full-stack)</t>
+        </is>
+      </c>
+      <c r="I440" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J440" t="n">
+        <v>4070</v>
+      </c>
+      <c r="K440" t="n">
+        <v>50875</v>
+      </c>
+      <c r="L440" t="b">
+        <v>1</v>
+      </c>
+      <c r="M440" t="inlineStr"/>
+      <c r="N440" t="inlineStr"/>
+      <c r="O440" t="n">
+        <v>4239.583333333333</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="2" t="n">
+        <v>44247.4519371412</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E441" t="n">
+        <v>4</v>
+      </c>
+      <c r="F441" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G441" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H441" t="inlineStr">
+        <is>
+          <t>Fullstack developer</t>
+        </is>
+      </c>
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J441" t="n">
+        <v>3200</v>
+      </c>
+      <c r="K441" t="n">
+        <v>41000</v>
+      </c>
+      <c r="L441" t="b">
+        <v>0</v>
+      </c>
+      <c r="M441" t="inlineStr">
+        <is>
+          <t>Futurice</t>
+        </is>
+      </c>
+      <c r="N441" t="inlineStr"/>
+      <c r="O441" t="n">
+        <v>3416.666666666667</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="2" t="n">
+        <v>44247.54319644676</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Jyväskylä</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E442" t="n">
+        <v>16</v>
+      </c>
+      <c r="F442" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G442" t="n">
+        <v>1</v>
+      </c>
+      <c r="H442" t="inlineStr">
+        <is>
+          <t>full-stack ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I442" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J442" t="n">
+        <v>4850</v>
+      </c>
+      <c r="K442" t="n">
+        <v>60500</v>
+      </c>
+      <c r="L442" t="b">
+        <v>1</v>
+      </c>
+      <c r="M442" t="inlineStr"/>
+      <c r="N442" t="inlineStr"/>
+      <c r="O442" t="n">
+        <v>5041.666666666667</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="2" t="n">
+        <v>44247.59054137731</v>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E443" t="n">
+        <v>13</v>
+      </c>
+      <c r="F443" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G443" t="n">
+        <v>1</v>
+      </c>
+      <c r="H443" t="inlineStr">
+        <is>
+          <t>full-stack</t>
+        </is>
+      </c>
+      <c r="I443" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J443" t="n">
+        <v>7500</v>
+      </c>
+      <c r="K443" t="n">
+        <v>93750</v>
+      </c>
+      <c r="L443" t="b">
+        <v>1</v>
+      </c>
+      <c r="M443" t="inlineStr">
+        <is>
+          <t>Mavericks</t>
+        </is>
+      </c>
+      <c r="N443" t="inlineStr"/>
+      <c r="O443" t="n">
+        <v>7812.5</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="2" t="n">
+        <v>44247.7031254051</v>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Turku</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>51-55 v</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E444" t="n">
+        <v>25</v>
+      </c>
+      <c r="F444" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G444" t="n">
+        <v>1</v>
+      </c>
+      <c r="H444" t="inlineStr">
+        <is>
+          <t>Ohjelmistonkehittäjä</t>
+        </is>
+      </c>
+      <c r="I444" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J444" t="n">
+        <v>3980</v>
+      </c>
+      <c r="K444" t="n">
+        <v>49750</v>
+      </c>
+      <c r="L444" t="b">
+        <v>0</v>
+      </c>
+      <c r="M444" t="inlineStr"/>
+      <c r="N444" t="inlineStr"/>
+      <c r="O444" t="n">
+        <v>4145.833333333333</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="2" t="n">
+        <v>44247.75843981482</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Tallinna</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>41-45 v</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E445" t="n">
+        <v>24</v>
+      </c>
+      <c r="F445" t="inlineStr">
+        <is>
+          <t>Yrittäjä</t>
+        </is>
+      </c>
+      <c r="G445" t="n">
+        <v>1</v>
+      </c>
+      <c r="H445" t="inlineStr">
+        <is>
+          <t>CTO/Founder/Kooderi</t>
+        </is>
+      </c>
+      <c r="I445" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J445" t="n">
+        <v>12000</v>
+      </c>
+      <c r="K445" t="n">
+        <v>300000</v>
+      </c>
+      <c r="L445" t="b">
+        <v>1</v>
+      </c>
+      <c r="M445" t="inlineStr"/>
+      <c r="N445" t="inlineStr"/>
+      <c r="O445" t="n">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="2" t="n">
+        <v>44247.80978547454</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E446" t="n">
+        <v>8</v>
+      </c>
+      <c r="F446" t="inlineStr">
+        <is>
+          <t>Freelancer</t>
+        </is>
+      </c>
+      <c r="G446" t="inlineStr"/>
+      <c r="H446" t="inlineStr">
+        <is>
+          <t>Full-stack</t>
+        </is>
+      </c>
+      <c r="I446" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J446" t="inlineStr"/>
+      <c r="K446" t="n">
+        <v>130000</v>
+      </c>
+      <c r="L446" t="b">
+        <v>1</v>
+      </c>
+      <c r="M446" t="inlineStr"/>
+      <c r="N446" t="inlineStr"/>
+      <c r="O446" t="n">
+        <v>10833.33333333333</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="2" t="n">
+        <v>44247.87873675926</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E447" t="n">
+        <v>13</v>
+      </c>
+      <c r="F447" t="inlineStr">
+        <is>
+          <t>Freelancer</t>
+        </is>
+      </c>
+      <c r="G447" t="inlineStr"/>
+      <c r="H447" t="inlineStr">
+        <is>
+          <t>ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I447" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J447" t="inlineStr"/>
+      <c r="K447" t="n">
+        <v>165000</v>
+      </c>
+      <c r="L447" t="b">
+        <v>1</v>
+      </c>
+      <c r="M447" t="inlineStr"/>
+      <c r="N447" t="inlineStr"/>
+      <c r="O447" t="n">
+        <v>13750</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="2" t="n">
+        <v>44247.88749210648</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E448" t="n">
+        <v>10</v>
+      </c>
+      <c r="F448" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G448" t="n">
+        <v>1</v>
+      </c>
+      <c r="H448" t="inlineStr">
+        <is>
+          <t>Software Architect</t>
+        </is>
+      </c>
+      <c r="I448" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J448" t="n">
+        <v>8000</v>
+      </c>
+      <c r="K448" t="n">
+        <v>100000</v>
+      </c>
+      <c r="L448" t="b">
+        <v>1</v>
+      </c>
+      <c r="M448" t="inlineStr">
+        <is>
+          <t>Compile Oy</t>
+        </is>
+      </c>
+      <c r="N448" t="inlineStr"/>
+      <c r="O448" t="n">
+        <v>8333.333333333334</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="2" t="n">
+        <v>44247.95472815972</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E449" t="n">
+        <v>7</v>
+      </c>
+      <c r="F449" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G449" t="n">
+        <v>1</v>
+      </c>
+      <c r="H449" t="inlineStr">
+        <is>
+          <t>Project manager</t>
+        </is>
+      </c>
+      <c r="I449" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J449" t="n">
+        <v>3800</v>
+      </c>
+      <c r="K449" t="n">
+        <v>47500</v>
+      </c>
+      <c r="L449" t="b">
+        <v>0</v>
+      </c>
+      <c r="M449" t="inlineStr"/>
+      <c r="N449" t="inlineStr"/>
+      <c r="O449" t="n">
+        <v>3958.333333333333</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="2" t="n">
+        <v>44248.49304268519</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E450" t="n">
+        <v>5</v>
+      </c>
+      <c r="F450" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G450" t="n">
+        <v>1</v>
+      </c>
+      <c r="H450" t="inlineStr">
+        <is>
+          <t>full-stack</t>
+        </is>
+      </c>
+      <c r="I450" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J450" t="n">
+        <v>5100</v>
+      </c>
+      <c r="K450" t="n">
+        <v>64000</v>
+      </c>
+      <c r="L450" t="b">
+        <v>1</v>
+      </c>
+      <c r="M450" t="inlineStr"/>
+      <c r="N450" t="inlineStr"/>
+      <c r="O450" t="n">
+        <v>5333.333333333333</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="2" t="n">
+        <v>44248.55438332176</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>41-45 v</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E451" t="n">
+        <v>10</v>
+      </c>
+      <c r="F451" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G451" t="n">
+        <v>1</v>
+      </c>
+      <c r="H451" t="inlineStr">
+        <is>
+          <t>Cloud Architect</t>
+        </is>
+      </c>
+      <c r="I451" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J451" t="n">
+        <v>5000</v>
+      </c>
+      <c r="K451" t="n">
+        <v>62500</v>
+      </c>
+      <c r="L451" t="b">
+        <v>0</v>
+      </c>
+      <c r="M451" t="inlineStr">
+        <is>
+          <t>Konsulttitalo</t>
+        </is>
+      </c>
+      <c r="N451" t="inlineStr"/>
+      <c r="O451" t="n">
+        <v>5208.333333333333</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="2" t="n">
+        <v>44248.71464697917</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E452" t="n">
+        <v>10</v>
+      </c>
+      <c r="F452" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G452" t="n">
+        <v>1</v>
+      </c>
+      <c r="H452" t="inlineStr">
+        <is>
+          <t>data engineering, team lead</t>
+        </is>
+      </c>
+      <c r="I452" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J452" t="n">
+        <v>5300</v>
+      </c>
+      <c r="K452" t="n">
+        <v>71500</v>
+      </c>
+      <c r="L452" t="b">
+        <v>0</v>
+      </c>
+      <c r="M452" t="inlineStr"/>
+      <c r="N452" t="inlineStr"/>
+      <c r="O452" t="n">
+        <v>5958.333333333333</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="2" t="n">
+        <v>44248.77370258102</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>21-25 v</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E453" t="n">
+        <v>1</v>
+      </c>
+      <c r="F453" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G453" t="n">
+        <v>1</v>
+      </c>
+      <c r="H453" t="inlineStr">
+        <is>
+          <t>Frontend</t>
+        </is>
+      </c>
+      <c r="I453" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J453" t="n">
+        <v>2600</v>
+      </c>
+      <c r="K453" t="n">
+        <v>31200</v>
+      </c>
+      <c r="L453" t="b">
+        <v>0</v>
+      </c>
+      <c r="M453" t="inlineStr"/>
+      <c r="N453" t="inlineStr"/>
+      <c r="O453" t="n">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="2" t="n">
+        <v>44248.96108387732</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E454" t="n">
+        <v>22</v>
+      </c>
+      <c r="F454" t="inlineStr">
+        <is>
+          <t>Yrittäjä</t>
+        </is>
+      </c>
+      <c r="G454" t="n">
+        <v>1</v>
+      </c>
+      <c r="H454" t="inlineStr">
+        <is>
+          <t>Full-stack</t>
+        </is>
+      </c>
+      <c r="I454" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J454" t="n">
+        <v>5000</v>
+      </c>
+      <c r="K454" t="n">
+        <v>85000</v>
+      </c>
+      <c r="L454" t="b">
+        <v>1</v>
+      </c>
+      <c r="M454" t="inlineStr"/>
+      <c r="N454" t="inlineStr"/>
+      <c r="O454" t="n">
+        <v>7083.333333333333</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="2" t="n">
+        <v>44249.31470427084</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Hämeenlinna</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr"/>
+      <c r="E455" t="n">
+        <v>5</v>
+      </c>
+      <c r="F455" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G455" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H455" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I455" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J455" t="n">
+        <v>2400</v>
+      </c>
+      <c r="K455" t="n">
+        <v>25000</v>
+      </c>
+      <c r="L455" t="b">
+        <v>0</v>
+      </c>
+      <c r="M455" t="inlineStr"/>
+      <c r="N455" t="inlineStr"/>
+      <c r="O455" t="n">
+        <v>2083.333333333333</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="2" t="n">
+        <v>44249.32453216436</v>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E456" t="n">
+        <v>12</v>
+      </c>
+      <c r="F456" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G456" t="n">
+        <v>1</v>
+      </c>
+      <c r="H456" t="inlineStr">
+        <is>
+          <t>Sovelluskehittäjä</t>
+        </is>
+      </c>
+      <c r="I456" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J456" t="n">
+        <v>6000</v>
+      </c>
+      <c r="K456" t="n">
+        <v>75000</v>
+      </c>
+      <c r="L456" t="b">
+        <v>0</v>
+      </c>
+      <c r="M456" t="inlineStr"/>
+      <c r="N456" t="inlineStr">
+        <is>
+          <t>Pieni firma ja paljon hattuja päässä. Palkka on hyvä, mutta ei korvaa stressiä ja painetta.</t>
+        </is>
+      </c>
+      <c r="O456" t="n">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="2" t="n">
+        <v>44249.40915908565</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Lontoo</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E457" t="n">
+        <v>17</v>
+      </c>
+      <c r="F457" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G457" t="n">
+        <v>1</v>
+      </c>
+      <c r="H457" t="inlineStr">
+        <is>
+          <t>CTO</t>
+        </is>
+      </c>
+      <c r="I457" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J457" t="n">
+        <v>8500</v>
+      </c>
+      <c r="K457" t="n">
+        <v>200000</v>
+      </c>
+      <c r="L457" t="b">
+        <v>1</v>
+      </c>
+      <c r="M457" t="inlineStr"/>
+      <c r="N457" t="inlineStr"/>
+      <c r="O457" t="n">
+        <v>16666.66666666667</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="2" t="n">
+        <v>44249.41863556713</v>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E458" t="n">
+        <v>3</v>
+      </c>
+      <c r="F458" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G458" t="n">
+        <v>1</v>
+      </c>
+      <c r="H458" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I458" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J458" t="n">
+        <v>3200</v>
+      </c>
+      <c r="K458" t="n">
+        <v>40000</v>
+      </c>
+      <c r="L458" t="b">
+        <v>0</v>
+      </c>
+      <c r="M458" t="inlineStr">
+        <is>
+          <t>Siili Solutions Oyj</t>
+        </is>
+      </c>
+      <c r="N458" t="inlineStr"/>
+      <c r="O458" t="n">
+        <v>3333.333333333333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@ac933d101db16236a47b0eb511fbfd41125f9974 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O461"/>
+  <dimension ref="A1:O469"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26018,6 +26018,450 @@
         <v>8333.333333333334</v>
       </c>
     </row>
+    <row r="462">
+      <c r="A462" s="2" t="n">
+        <v>44249.53087737269</v>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E462" t="n">
+        <v>15</v>
+      </c>
+      <c r="F462" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G462" t="n">
+        <v>1</v>
+      </c>
+      <c r="H462" t="inlineStr">
+        <is>
+          <t>fullstack-ohjelmistokehittä / arkkitehti / pilviveikko</t>
+        </is>
+      </c>
+      <c r="I462" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J462" t="n">
+        <v>5700</v>
+      </c>
+      <c r="K462" t="n">
+        <v>70000</v>
+      </c>
+      <c r="L462" t="b">
+        <v>1</v>
+      </c>
+      <c r="M462" t="inlineStr"/>
+      <c r="N462" t="inlineStr"/>
+      <c r="O462" t="n">
+        <v>5833.333333333333</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="2" t="n">
+        <v>44249.53103743056</v>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Oulu</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E463" t="n">
+        <v>7</v>
+      </c>
+      <c r="F463" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G463" t="n">
+        <v>1</v>
+      </c>
+      <c r="H463" t="inlineStr">
+        <is>
+          <t>Backend</t>
+        </is>
+      </c>
+      <c r="I463" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J463" t="n">
+        <v>3800</v>
+      </c>
+      <c r="K463" t="n">
+        <v>47500</v>
+      </c>
+      <c r="L463" t="b">
+        <v>1</v>
+      </c>
+      <c r="M463" t="inlineStr"/>
+      <c r="N463" t="inlineStr"/>
+      <c r="O463" t="n">
+        <v>3958.333333333333</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="2" t="n">
+        <v>44249.53438325231</v>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E464" t="n">
+        <v>5</v>
+      </c>
+      <c r="F464" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G464" t="n">
+        <v>1</v>
+      </c>
+      <c r="H464" t="inlineStr">
+        <is>
+          <t>Mobiilikehittäjä</t>
+        </is>
+      </c>
+      <c r="I464" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J464" t="n">
+        <v>4500</v>
+      </c>
+      <c r="K464" t="n">
+        <v>56250</v>
+      </c>
+      <c r="L464" t="b">
+        <v>1</v>
+      </c>
+      <c r="M464" t="inlineStr"/>
+      <c r="N464" t="inlineStr"/>
+      <c r="O464" t="n">
+        <v>4687.5</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="2" t="n">
+        <v>44249.5357290625</v>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Oulu</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E465" t="n">
+        <v>5</v>
+      </c>
+      <c r="F465" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G465" t="n">
+        <v>1</v>
+      </c>
+      <c r="H465" t="inlineStr">
+        <is>
+          <t>Web developer</t>
+        </is>
+      </c>
+      <c r="I465" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J465" t="n">
+        <v>3000</v>
+      </c>
+      <c r="K465" t="n">
+        <v>37500</v>
+      </c>
+      <c r="L465" t="b">
+        <v>0</v>
+      </c>
+      <c r="M465" t="inlineStr"/>
+      <c r="N465" t="inlineStr">
+        <is>
+          <t>Kokemusta kokonaisuudessaan 7v, mutta siitä reilut kaksi vuotta lasten kanssa kotona koodaamatta.</t>
+        </is>
+      </c>
+      <c r="O465" t="n">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="2" t="n">
+        <v>44249.53759880787</v>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E466" t="n">
+        <v>9</v>
+      </c>
+      <c r="F466" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G466" t="n">
+        <v>1</v>
+      </c>
+      <c r="H466" t="inlineStr">
+        <is>
+          <t>Tuotepäällikkö</t>
+        </is>
+      </c>
+      <c r="I466" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J466" t="n">
+        <v>5500</v>
+      </c>
+      <c r="K466" t="n">
+        <v>82500</v>
+      </c>
+      <c r="L466" t="b">
+        <v>1</v>
+      </c>
+      <c r="M466" t="inlineStr"/>
+      <c r="N466" t="inlineStr"/>
+      <c r="O466" t="n">
+        <v>6875</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="2" t="n">
+        <v>44249.54394976852</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E467" t="n">
+        <v>5</v>
+      </c>
+      <c r="F467" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G467" t="n">
+        <v>1</v>
+      </c>
+      <c r="H467" t="inlineStr">
+        <is>
+          <t>Lead front end dev</t>
+        </is>
+      </c>
+      <c r="I467" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J467" t="n">
+        <v>4200</v>
+      </c>
+      <c r="K467" t="n">
+        <v>50000</v>
+      </c>
+      <c r="L467" t="b">
+        <v>1</v>
+      </c>
+      <c r="M467" t="inlineStr"/>
+      <c r="N467" t="inlineStr"/>
+      <c r="O467" t="n">
+        <v>4166.666666666667</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="2" t="n">
+        <v>44249.56513866898</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>26-30 v</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E468" t="n">
+        <v>0</v>
+      </c>
+      <c r="F468" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G468" t="n">
+        <v>1</v>
+      </c>
+      <c r="H468" t="inlineStr">
+        <is>
+          <t>harjoittelija</t>
+        </is>
+      </c>
+      <c r="I468" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J468" t="n">
+        <v>2200</v>
+      </c>
+      <c r="K468" t="n">
+        <v>27500</v>
+      </c>
+      <c r="L468" t="b">
+        <v>0</v>
+      </c>
+      <c r="M468" t="inlineStr"/>
+      <c r="N468" t="inlineStr"/>
+      <c r="O468" t="n">
+        <v>2291.666666666667</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="2" t="n">
+        <v>44249.59106795139</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>EU</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E469" t="n">
+        <v>8</v>
+      </c>
+      <c r="F469" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G469" t="n">
+        <v>1</v>
+      </c>
+      <c r="H469" t="inlineStr">
+        <is>
+          <t>Senior Backend Developer</t>
+        </is>
+      </c>
+      <c r="I469" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J469" t="n">
+        <v>4800</v>
+      </c>
+      <c r="K469" t="n">
+        <v>59000</v>
+      </c>
+      <c r="L469" t="b">
+        <v>0</v>
+      </c>
+      <c r="M469" t="inlineStr"/>
+      <c r="N469" t="inlineStr"/>
+      <c r="O469" t="n">
+        <v>4916.666666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@f1e90adddec639bad8b9ea139b07a431e87a4ebd 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O469"/>
+  <dimension ref="A1:O470"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26462,6 +26462,61 @@
         <v>4916.666666666667</v>
       </c>
     </row>
+    <row r="470">
+      <c r="A470" s="2" t="n">
+        <v>44249.79080961805</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>41-45 v</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E470" t="n">
+        <v>15</v>
+      </c>
+      <c r="F470" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G470" t="n">
+        <v>1</v>
+      </c>
+      <c r="H470" t="inlineStr">
+        <is>
+          <t>Teknologiajohtaja</t>
+        </is>
+      </c>
+      <c r="I470" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J470" t="n">
+        <v>12000</v>
+      </c>
+      <c r="K470" t="n">
+        <v>220000</v>
+      </c>
+      <c r="L470" t="b">
+        <v>1</v>
+      </c>
+      <c r="M470" t="inlineStr"/>
+      <c r="N470" t="inlineStr"/>
+      <c r="O470" t="n">
+        <v>18333.33333333333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@b54ca2ceeae6c692adf0d71771640adee8724d19 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O493"/>
+  <dimension ref="A1:O494"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>Digia Oyj</t>
+          <t>Digiaj</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>Compile Oy</t>
+          <t>Compile</t>
         </is>
       </c>
       <c r="N64" t="inlineStr"/>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>Gofore Oyj</t>
+          <t>Goforej</t>
         </is>
       </c>
       <c r="N101" t="inlineStr"/>
@@ -6922,7 +6922,7 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
-          <t>Verkkokauppa.com Oyj</t>
+          <t>Verkkokauppa.comj</t>
         </is>
       </c>
       <c r="N117" t="inlineStr"/>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>SurviveJS Oy</t>
+          <t>SurviveJS</t>
         </is>
       </c>
       <c r="N119" t="inlineStr"/>
@@ -8725,7 +8725,7 @@
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>Digitoimisto Dude Oy</t>
+          <t>Digitoimisto Dude</t>
         </is>
       </c>
       <c r="N150" t="inlineStr"/>
@@ -12601,7 +12601,7 @@
       </c>
       <c r="M220" t="inlineStr">
         <is>
-          <t>Gofore Oyj</t>
+          <t>Goforej</t>
         </is>
       </c>
       <c r="N220" t="inlineStr"/>
@@ -13157,7 +13157,7 @@
       </c>
       <c r="M230" t="inlineStr">
         <is>
-          <t>Columbia Road Oy</t>
+          <t>Columbia Road</t>
         </is>
       </c>
       <c r="N230" t="inlineStr"/>
@@ -15855,7 +15855,7 @@
       </c>
       <c r="M278" t="inlineStr">
         <is>
-          <t>Zure Oy</t>
+          <t>Zure</t>
         </is>
       </c>
       <c r="N278" t="inlineStr"/>
@@ -16187,7 +16187,7 @@
       </c>
       <c r="M284" t="inlineStr">
         <is>
-          <t>Telia Cygate Oy</t>
+          <t>Telia Cygate</t>
         </is>
       </c>
       <c r="N284" t="inlineStr"/>
@@ -17576,7 +17576,7 @@
       <c r="L309" t="inlineStr"/>
       <c r="M309" t="inlineStr">
         <is>
-          <t xml:space="preserve">KVTES-alainen kunnan omistama oy </t>
+          <t xml:space="preserve">KVTES-alainen kunnan omistama </t>
         </is>
       </c>
       <c r="N309" t="inlineStr">
@@ -18360,7 +18360,7 @@
       <c r="L323" t="inlineStr"/>
       <c r="M323" t="inlineStr">
         <is>
-          <t xml:space="preserve">KVTES-alainen kunnan omistama oy </t>
+          <t xml:space="preserve">KVTES-alainen kunnan omistama </t>
         </is>
       </c>
       <c r="N323" t="inlineStr">
@@ -21733,7 +21733,7 @@
       </c>
       <c r="M384" t="inlineStr">
         <is>
-          <t>Rare Agency Oy</t>
+          <t>Rare Agency</t>
         </is>
       </c>
       <c r="N384" t="inlineStr"/>
@@ -24662,7 +24662,7 @@
       </c>
       <c r="M437" t="inlineStr">
         <is>
-          <t>Bitwise Oy</t>
+          <t>Bitwise</t>
         </is>
       </c>
       <c r="N437" t="inlineStr"/>
@@ -24776,7 +24776,7 @@
       </c>
       <c r="M439" t="inlineStr">
         <is>
-          <t>Mavericks Software Oy</t>
+          <t>Mavericks Software</t>
         </is>
       </c>
       <c r="N439" t="inlineStr"/>
@@ -25275,7 +25275,7 @@
       </c>
       <c r="M448" t="inlineStr">
         <is>
-          <t>Compile Oy</t>
+          <t>Compile</t>
         </is>
       </c>
       <c r="N448" t="inlineStr"/>
@@ -25833,7 +25833,7 @@
       </c>
       <c r="M458" t="inlineStr">
         <is>
-          <t>Siili Solutions Oyj</t>
+          <t>Siili Solutionsj</t>
         </is>
       </c>
       <c r="N458" t="inlineStr"/>
@@ -27118,7 +27118,7 @@
       </c>
       <c r="M481" t="inlineStr">
         <is>
-          <t>Tuspe Design Oy</t>
+          <t>Tuspe Design</t>
         </is>
       </c>
       <c r="N481" t="inlineStr"/>
@@ -27782,6 +27782,65 @@
         <v>5833.333333333333</v>
       </c>
     </row>
+    <row r="494">
+      <c r="A494" s="2" t="n">
+        <v>44253.51133907407</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>36-40 v</t>
+        </is>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E494" t="n">
+        <v>15</v>
+      </c>
+      <c r="F494" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G494" t="n">
+        <v>1</v>
+      </c>
+      <c r="H494" t="inlineStr">
+        <is>
+          <t>Ohjelmistosuunnittelija</t>
+        </is>
+      </c>
+      <c r="I494" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J494" t="n">
+        <v>4300</v>
+      </c>
+      <c r="K494" t="n">
+        <v>53750</v>
+      </c>
+      <c r="L494" t="b">
+        <v>0</v>
+      </c>
+      <c r="M494" t="inlineStr">
+        <is>
+          <t>Gofore</t>
+        </is>
+      </c>
+      <c r="N494" t="inlineStr"/>
+      <c r="O494" t="n">
+        <v>4479.166666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ koodiklinikka/palkkakysely@65e3480a78d0e7b66e06c5d3650c2a17ec14cd1c 🚀
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O494"/>
+  <dimension ref="A1:O498"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27841,6 +27841,228 @@
         <v>4479.166666666667</v>
       </c>
     </row>
+    <row r="495">
+      <c r="A495" s="2" t="n">
+        <v>44253.51518861111</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Tampere</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E495" t="n">
+        <v>11</v>
+      </c>
+      <c r="F495" t="inlineStr">
+        <is>
+          <t>Freelancer</t>
+        </is>
+      </c>
+      <c r="G495" t="n">
+        <v>1</v>
+      </c>
+      <c r="H495" t="inlineStr">
+        <is>
+          <t>frontend</t>
+        </is>
+      </c>
+      <c r="I495" t="inlineStr">
+        <is>
+          <t>Etä</t>
+        </is>
+      </c>
+      <c r="J495" t="inlineStr"/>
+      <c r="K495" t="n">
+        <v>157300</v>
+      </c>
+      <c r="L495" t="b">
+        <v>1</v>
+      </c>
+      <c r="M495" t="inlineStr"/>
+      <c r="N495" t="inlineStr"/>
+      <c r="O495" t="n">
+        <v>13108.33333333333</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="2" t="n">
+        <v>44253.53237736111</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E496" t="n">
+        <v>11</v>
+      </c>
+      <c r="F496" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G496" t="n">
+        <v>1</v>
+      </c>
+      <c r="H496" t="inlineStr">
+        <is>
+          <t>Arkkitehti</t>
+        </is>
+      </c>
+      <c r="I496" t="inlineStr">
+        <is>
+          <t>Toimisto</t>
+        </is>
+      </c>
+      <c r="J496" t="n">
+        <v>6500</v>
+      </c>
+      <c r="K496" t="n">
+        <v>81250</v>
+      </c>
+      <c r="L496" t="b">
+        <v>1</v>
+      </c>
+      <c r="M496" t="inlineStr">
+        <is>
+          <t>Siili</t>
+        </is>
+      </c>
+      <c r="N496" t="inlineStr"/>
+      <c r="O496" t="n">
+        <v>6770.833333333333</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="2" t="n">
+        <v>44253.53294115741</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>nainen</t>
+        </is>
+      </c>
+      <c r="E497" t="n">
+        <v>3</v>
+      </c>
+      <c r="F497" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G497" t="n">
+        <v>1</v>
+      </c>
+      <c r="H497" t="inlineStr">
+        <is>
+          <t>Full-stack</t>
+        </is>
+      </c>
+      <c r="I497" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J497" t="n">
+        <v>3800</v>
+      </c>
+      <c r="K497" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L497" t="b">
+        <v>0</v>
+      </c>
+      <c r="M497" t="inlineStr"/>
+      <c r="N497" t="inlineStr"/>
+      <c r="O497" t="inlineStr"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="2" t="n">
+        <v>44253.55874591435</v>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>PK-Seutu</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>31-35 v</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>mies</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr"/>
+      <c r="F498" t="inlineStr">
+        <is>
+          <t>Työntekijä / palkollinen</t>
+        </is>
+      </c>
+      <c r="G498" t="n">
+        <v>1</v>
+      </c>
+      <c r="H498" t="inlineStr">
+        <is>
+          <t>Ohjelmistokehittäjä</t>
+        </is>
+      </c>
+      <c r="I498" t="inlineStr">
+        <is>
+          <t>50/50</t>
+        </is>
+      </c>
+      <c r="J498" t="inlineStr"/>
+      <c r="K498" t="n">
+        <v>75000</v>
+      </c>
+      <c r="L498" t="b">
+        <v>1</v>
+      </c>
+      <c r="M498" t="inlineStr">
+        <is>
+          <t>Vincit</t>
+        </is>
+      </c>
+      <c r="N498" t="inlineStr"/>
+      <c r="O498" t="n">
+        <v>6250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>